<commit_message>
Add support for Balsamic-UMI
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1604.14.rml.xlsx
+++ b/tests/fixtures/orderforms/1604.14.rml.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik.grenfeldt/Documents/GitHub/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42061A2-E9BA-D046-918D-1E0625D4DDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9480635E-E183-D349-B6BC-E6DFB6E392D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DD23Ae9qJhC5962EjDbkniUmlV7E5os8o2LjlcGfzEUj5yt22g+hDV+kLwtoma25o0rM2RxA7HL+8jzO4x2tWA==" workbookSaltValue="3wB72j/MgB4sBrqBZE4epQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="-19400" windowWidth="27840" windowHeight="17500" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -6626,15 +6626,6 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -6648,6 +6639,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="279">
@@ -7415,7 +7415,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -7459,7 +7459,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -7486,8 +7486,8 @@
   </sheetPr>
   <dimension ref="A1:Z399"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F9" zoomScale="116" zoomScaleNormal="116" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="116" zoomScaleNormal="116" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7744,34 +7744,34 @@
       <c r="Z8" s="128"/>
     </row>
     <row r="9" spans="1:26" s="131" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="169" t="s">
+      <c r="A9" s="173" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="170"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="170"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="170"/>
-      <c r="K9" s="170"/>
-      <c r="L9" s="171"/>
+      <c r="B9" s="174"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="174"/>
+      <c r="E9" s="174"/>
+      <c r="F9" s="174"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="174"/>
+      <c r="J9" s="174"/>
+      <c r="K9" s="174"/>
+      <c r="L9" s="175"/>
       <c r="M9" s="107"/>
-      <c r="N9" s="169" t="s">
+      <c r="N9" s="173" t="s">
         <v>89</v>
       </c>
-      <c r="O9" s="171"/>
+      <c r="O9" s="175"/>
       <c r="P9" s="107"/>
       <c r="Q9" s="23" t="s">
         <v>1077</v>
       </c>
       <c r="R9" s="117"/>
-      <c r="S9" s="169" t="s">
+      <c r="S9" s="173" t="s">
         <v>316</v>
       </c>
-      <c r="T9" s="171"/>
+      <c r="T9" s="175"/>
       <c r="U9" s="115"/>
       <c r="V9" s="103"/>
       <c r="W9" s="130"/>
@@ -7779,7 +7779,7 @@
       <c r="Y9" s="130"/>
       <c r="Z9" s="130"/>
     </row>
-    <row r="10" spans="1:26" s="131" customFormat="1" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" s="131" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="74" t="s">
         <v>0</v>
       </c>
@@ -7809,7 +7809,7 @@
       <c r="Y10" s="130"/>
       <c r="Z10" s="130"/>
     </row>
-    <row r="11" spans="1:26" s="133" customFormat="1" ht="41" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" s="133" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="75" t="s">
         <v>85</v>
       </c>
@@ -7870,7 +7870,7 @@
       <c r="Y11" s="136"/>
       <c r="Z11" s="137"/>
     </row>
-    <row r="12" spans="1:26" s="141" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" s="141" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="76" t="s">
         <v>1</v>
       </c>
@@ -7961,7 +7961,7 @@
       <c r="Y13" s="144"/>
       <c r="Z13" s="145"/>
     </row>
-    <row r="14" spans="1:26" s="141" customFormat="1" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" s="141" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="77" t="s">
         <v>2</v>
       </c>
@@ -7997,10 +7997,10 @@
       <c r="B15" s="78" t="s">
         <v>1583</v>
       </c>
-      <c r="C15" s="172" t="s">
+      <c r="C15" s="169" t="s">
         <v>420</v>
       </c>
-      <c r="D15" s="174" t="s">
+      <c r="D15" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E15" s="56" t="s">
@@ -8021,7 +8021,7 @@
       <c r="J15" s="58">
         <v>2</v>
       </c>
-      <c r="K15" s="175" t="s">
+      <c r="K15" s="172" t="s">
         <v>870</v>
       </c>
       <c r="L15" s="58">
@@ -8059,10 +8059,10 @@
       <c r="B16" s="78" t="s">
         <v>1585</v>
       </c>
-      <c r="C16" s="172" t="s">
+      <c r="C16" s="169" t="s">
         <v>421</v>
       </c>
-      <c r="D16" s="174" t="s">
+      <c r="D16" s="171" t="s">
         <v>419</v>
       </c>
       <c r="E16" s="56" t="s">
@@ -8083,7 +8083,7 @@
       <c r="J16" s="58">
         <v>2</v>
       </c>
-      <c r="K16" s="175" t="s">
+      <c r="K16" s="172" t="s">
         <v>79</v>
       </c>
       <c r="L16" s="58">
@@ -8113,10 +8113,10 @@
       <c r="B17" s="78" t="s">
         <v>1587</v>
       </c>
-      <c r="C17" s="172" t="s">
+      <c r="C17" s="169" t="s">
         <v>422</v>
       </c>
-      <c r="D17" s="174" t="s">
+      <c r="D17" s="171" t="s">
         <v>865</v>
       </c>
       <c r="E17" s="56" t="s">
@@ -8135,7 +8135,7 @@
       <c r="J17" s="58">
         <v>2</v>
       </c>
-      <c r="K17" s="174" t="s">
+      <c r="K17" s="171" t="s">
         <v>767</v>
       </c>
       <c r="L17" s="58">
@@ -8165,10 +8165,10 @@
       <c r="B18" s="78" t="s">
         <v>1589</v>
       </c>
-      <c r="C18" s="172" t="s">
+      <c r="C18" s="169" t="s">
         <v>423</v>
       </c>
-      <c r="D18" s="174" t="s">
+      <c r="D18" s="171" t="s">
         <v>871</v>
       </c>
       <c r="E18" s="56" t="s">
@@ -8187,7 +8187,7 @@
       <c r="J18" s="58">
         <v>2</v>
       </c>
-      <c r="K18" s="174" t="s">
+      <c r="K18" s="171" t="s">
         <v>1176</v>
       </c>
       <c r="L18" s="58">
@@ -8217,10 +8217,10 @@
       <c r="B19" s="78" t="s">
         <v>1591</v>
       </c>
-      <c r="C19" s="172" t="s">
+      <c r="C19" s="169" t="s">
         <v>424</v>
       </c>
-      <c r="D19" s="174" t="s">
+      <c r="D19" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E19" s="56" t="s">
@@ -8239,7 +8239,7 @@
       <c r="J19" s="58">
         <v>2</v>
       </c>
-      <c r="K19" s="174" t="s">
+      <c r="K19" s="171" t="s">
         <v>876</v>
       </c>
       <c r="L19" s="58">
@@ -8269,10 +8269,10 @@
       <c r="B20" s="78" t="s">
         <v>1593</v>
       </c>
-      <c r="C20" s="172" t="s">
+      <c r="C20" s="169" t="s">
         <v>425</v>
       </c>
-      <c r="D20" s="174" t="s">
+      <c r="D20" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E20" s="56" t="s">
@@ -8291,7 +8291,7 @@
       <c r="J20" s="58">
         <v>2</v>
       </c>
-      <c r="K20" s="174" t="s">
+      <c r="K20" s="171" t="s">
         <v>1177</v>
       </c>
       <c r="L20" s="58">
@@ -8321,10 +8321,10 @@
       <c r="B21" s="78" t="s">
         <v>1595</v>
       </c>
-      <c r="C21" s="172" t="s">
+      <c r="C21" s="169" t="s">
         <v>426</v>
       </c>
-      <c r="D21" s="174" t="s">
+      <c r="D21" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E21" s="56" t="s">
@@ -8343,7 +8343,7 @@
       <c r="J21" s="58">
         <v>2</v>
       </c>
-      <c r="K21" s="174" t="s">
+      <c r="K21" s="171" t="s">
         <v>1183</v>
       </c>
       <c r="L21" s="58">
@@ -8373,10 +8373,10 @@
       <c r="B22" s="78" t="s">
         <v>1597</v>
       </c>
-      <c r="C22" s="172" t="s">
+      <c r="C22" s="169" t="s">
         <v>427</v>
       </c>
-      <c r="D22" s="174" t="s">
+      <c r="D22" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E22" s="56" t="s">
@@ -8395,7 +8395,7 @@
       <c r="J22" s="58">
         <v>2</v>
       </c>
-      <c r="K22" s="174" t="s">
+      <c r="K22" s="171" t="s">
         <v>1384</v>
       </c>
       <c r="L22" s="58">
@@ -8425,10 +8425,10 @@
       <c r="B23" s="78" t="s">
         <v>1599</v>
       </c>
-      <c r="C23" s="172" t="s">
+      <c r="C23" s="169" t="s">
         <v>428</v>
       </c>
-      <c r="D23" s="174" t="s">
+      <c r="D23" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E23" s="56" t="s">
@@ -8447,7 +8447,7 @@
       <c r="J23" s="58">
         <v>2</v>
       </c>
-      <c r="K23" s="174" t="s">
+      <c r="K23" s="171" t="s">
         <v>1385</v>
       </c>
       <c r="L23" s="58">
@@ -8477,10 +8477,10 @@
       <c r="B24" s="78" t="s">
         <v>1601</v>
       </c>
-      <c r="C24" s="172" t="s">
+      <c r="C24" s="169" t="s">
         <v>429</v>
       </c>
-      <c r="D24" s="174" t="s">
+      <c r="D24" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E24" s="56" t="s">
@@ -8499,7 +8499,7 @@
       <c r="J24" s="58">
         <v>2</v>
       </c>
-      <c r="K24" s="174" t="s">
+      <c r="K24" s="171" t="s">
         <v>974</v>
       </c>
       <c r="L24" s="58">
@@ -8529,10 +8529,10 @@
       <c r="B25" s="78" t="s">
         <v>1603</v>
       </c>
-      <c r="C25" s="173" t="s">
+      <c r="C25" s="170" t="s">
         <v>430</v>
       </c>
-      <c r="D25" s="174" t="s">
+      <c r="D25" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E25" s="56" t="s">
@@ -8551,7 +8551,7 @@
       <c r="J25" s="58">
         <v>2</v>
       </c>
-      <c r="K25" s="175" t="s">
+      <c r="K25" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L25" s="58"/>
@@ -8579,10 +8579,10 @@
       <c r="B26" s="78" t="s">
         <v>1605</v>
       </c>
-      <c r="C26" s="173" t="s">
+      <c r="C26" s="170" t="s">
         <v>431</v>
       </c>
-      <c r="D26" s="174" t="s">
+      <c r="D26" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E26" s="56" t="s">
@@ -8601,7 +8601,7 @@
       <c r="J26" s="58">
         <v>2</v>
       </c>
-      <c r="K26" s="175" t="s">
+      <c r="K26" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L26" s="58"/>
@@ -8629,10 +8629,10 @@
       <c r="B27" s="78" t="s">
         <v>1607</v>
       </c>
-      <c r="C27" s="173" t="s">
+      <c r="C27" s="170" t="s">
         <v>432</v>
       </c>
-      <c r="D27" s="174" t="s">
+      <c r="D27" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E27" s="56" t="s">
@@ -8651,7 +8651,7 @@
       <c r="J27" s="58">
         <v>2</v>
       </c>
-      <c r="K27" s="175" t="s">
+      <c r="K27" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L27" s="58"/>
@@ -8679,10 +8679,10 @@
       <c r="B28" s="78" t="s">
         <v>1609</v>
       </c>
-      <c r="C28" s="173" t="s">
+      <c r="C28" s="170" t="s">
         <v>433</v>
       </c>
-      <c r="D28" s="174" t="s">
+      <c r="D28" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E28" s="56" t="s">
@@ -8701,7 +8701,7 @@
       <c r="J28" s="58">
         <v>2</v>
       </c>
-      <c r="K28" s="175" t="s">
+      <c r="K28" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L28" s="58"/>
@@ -8729,10 +8729,10 @@
       <c r="B29" s="78" t="s">
         <v>1611</v>
       </c>
-      <c r="C29" s="173" t="s">
+      <c r="C29" s="170" t="s">
         <v>434</v>
       </c>
-      <c r="D29" s="174" t="s">
+      <c r="D29" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E29" s="56" t="s">
@@ -8751,7 +8751,7 @@
       <c r="J29" s="58">
         <v>2</v>
       </c>
-      <c r="K29" s="175" t="s">
+      <c r="K29" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L29" s="58"/>
@@ -8779,10 +8779,10 @@
       <c r="B30" s="78" t="s">
         <v>1613</v>
       </c>
-      <c r="C30" s="173" t="s">
+      <c r="C30" s="170" t="s">
         <v>435</v>
       </c>
-      <c r="D30" s="174" t="s">
+      <c r="D30" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E30" s="56" t="s">
@@ -8801,7 +8801,7 @@
       <c r="J30" s="58">
         <v>2</v>
       </c>
-      <c r="K30" s="175" t="s">
+      <c r="K30" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L30" s="58"/>
@@ -8829,10 +8829,10 @@
       <c r="B31" s="78" t="s">
         <v>1615</v>
       </c>
-      <c r="C31" s="173" t="s">
+      <c r="C31" s="170" t="s">
         <v>436</v>
       </c>
-      <c r="D31" s="174" t="s">
+      <c r="D31" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E31" s="56" t="s">
@@ -8851,7 +8851,7 @@
       <c r="J31" s="58">
         <v>2</v>
       </c>
-      <c r="K31" s="175" t="s">
+      <c r="K31" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L31" s="58"/>
@@ -8879,10 +8879,10 @@
       <c r="B32" s="78" t="s">
         <v>1617</v>
       </c>
-      <c r="C32" s="173" t="s">
+      <c r="C32" s="170" t="s">
         <v>437</v>
       </c>
-      <c r="D32" s="174" t="s">
+      <c r="D32" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E32" s="56" t="s">
@@ -8901,7 +8901,7 @@
       <c r="J32" s="58">
         <v>2</v>
       </c>
-      <c r="K32" s="175" t="s">
+      <c r="K32" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L32" s="58"/>
@@ -8929,10 +8929,10 @@
       <c r="B33" s="78" t="s">
         <v>1619</v>
       </c>
-      <c r="C33" s="173" t="s">
+      <c r="C33" s="170" t="s">
         <v>438</v>
       </c>
-      <c r="D33" s="174" t="s">
+      <c r="D33" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E33" s="56" t="s">
@@ -8951,7 +8951,7 @@
       <c r="J33" s="58">
         <v>2</v>
       </c>
-      <c r="K33" s="175" t="s">
+      <c r="K33" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L33" s="58"/>
@@ -8979,10 +8979,10 @@
       <c r="B34" s="78" t="s">
         <v>1621</v>
       </c>
-      <c r="C34" s="173" t="s">
+      <c r="C34" s="170" t="s">
         <v>872</v>
       </c>
-      <c r="D34" s="174" t="s">
+      <c r="D34" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E34" s="56" t="s">
@@ -9001,7 +9001,7 @@
       <c r="J34" s="58">
         <v>2</v>
       </c>
-      <c r="K34" s="175" t="s">
+      <c r="K34" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L34" s="58"/>
@@ -9029,10 +9029,10 @@
       <c r="B35" s="78" t="s">
         <v>1623</v>
       </c>
-      <c r="C35" s="173" t="s">
+      <c r="C35" s="170" t="s">
         <v>873</v>
       </c>
-      <c r="D35" s="174" t="s">
+      <c r="D35" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E35" s="56" t="s">
@@ -9051,7 +9051,7 @@
       <c r="J35" s="58">
         <v>2</v>
       </c>
-      <c r="K35" s="175" t="s">
+      <c r="K35" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L35" s="58"/>
@@ -9079,10 +9079,10 @@
       <c r="B36" s="78" t="s">
         <v>1625</v>
       </c>
-      <c r="C36" s="173" t="s">
+      <c r="C36" s="170" t="s">
         <v>874</v>
       </c>
-      <c r="D36" s="174" t="s">
+      <c r="D36" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E36" s="56" t="s">
@@ -9101,7 +9101,7 @@
       <c r="J36" s="58">
         <v>2</v>
       </c>
-      <c r="K36" s="175" t="s">
+      <c r="K36" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L36" s="58"/>
@@ -9129,10 +9129,10 @@
       <c r="B37" s="78" t="s">
         <v>1627</v>
       </c>
-      <c r="C37" s="173" t="s">
+      <c r="C37" s="170" t="s">
         <v>875</v>
       </c>
-      <c r="D37" s="174" t="s">
+      <c r="D37" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E37" s="56" t="s">
@@ -9151,7 +9151,7 @@
       <c r="J37" s="58">
         <v>2</v>
       </c>
-      <c r="K37" s="175" t="s">
+      <c r="K37" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L37" s="58"/>
@@ -9179,10 +9179,10 @@
       <c r="B38" s="78" t="s">
         <v>1629</v>
       </c>
-      <c r="C38" s="173" t="s">
+      <c r="C38" s="170" t="s">
         <v>864</v>
       </c>
-      <c r="D38" s="174" t="s">
+      <c r="D38" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E38" s="56" t="s">
@@ -9201,7 +9201,7 @@
       <c r="J38" s="58">
         <v>2</v>
       </c>
-      <c r="K38" s="175" t="s">
+      <c r="K38" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L38" s="58"/>
@@ -9225,7 +9225,7 @@
     <row r="39" spans="1:26" s="151" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="100"/>
       <c r="B39" s="78"/>
-      <c r="C39" s="173" t="s">
+      <c r="C39" s="170" t="s">
         <v>1579</v>
       </c>
       <c r="D39" s="60"/>
@@ -9245,7 +9245,7 @@
       <c r="J39" s="58">
         <v>2</v>
       </c>
-      <c r="K39" s="175" t="s">
+      <c r="K39" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L39" s="58"/>
@@ -9269,7 +9269,7 @@
     <row r="40" spans="1:26" s="151" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="100"/>
       <c r="B40" s="78"/>
-      <c r="C40" s="173" t="s">
+      <c r="C40" s="170" t="s">
         <v>1580</v>
       </c>
       <c r="D40" s="60"/>
@@ -9289,7 +9289,7 @@
       <c r="J40" s="58">
         <v>2</v>
       </c>
-      <c r="K40" s="175" t="s">
+      <c r="K40" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L40" s="58"/>
@@ -20059,7 +20059,7 @@
       <c r="T399" s="163"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LcEW3xxqy8+uxIfecIYabamdN8eTKoPpDyQutSviBMF83dE15eAIw/7xf88mxehDeKVO0pK6Sirr6CzoHnWduw==" saltValue="phe6gu6JQS2q2aNlfVxepQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="N9:O9"/>

</xml_diff>

<commit_message>
Feat(Ordering): Support OF 1508:26 (#1466)
### Added:
* Add support for Balsamic-UMI
* Require subject-id
* Support bed for fastq and control for case orders
* Remove sample.time_point
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1604.14.rml.xlsx
+++ b/tests/fixtures/orderforms/1604.14.rml.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrik.grenfeldt/Documents/GitHub/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42061A2-E9BA-D046-918D-1E0625D4DDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9480635E-E183-D349-B6BC-E6DFB6E392D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DD23Ae9qJhC5962EjDbkniUmlV7E5os8o2LjlcGfzEUj5yt22g+hDV+kLwtoma25o0rM2RxA7HL+8jzO4x2tWA==" workbookSaltValue="3wB72j/MgB4sBrqBZE4epQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="-19400" windowWidth="27840" windowHeight="17500" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -6626,15 +6626,6 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -6648,6 +6639,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="279">
@@ -7415,7 +7415,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -7459,7 +7459,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -7486,8 +7486,8 @@
   </sheetPr>
   <dimension ref="A1:Z399"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F9" zoomScale="116" zoomScaleNormal="116" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="116" zoomScaleNormal="116" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7744,34 +7744,34 @@
       <c r="Z8" s="128"/>
     </row>
     <row r="9" spans="1:26" s="131" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="169" t="s">
+      <c r="A9" s="173" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="170"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="170"/>
-      <c r="E9" s="170"/>
-      <c r="F9" s="170"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="170"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="170"/>
-      <c r="K9" s="170"/>
-      <c r="L9" s="171"/>
+      <c r="B9" s="174"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="174"/>
+      <c r="E9" s="174"/>
+      <c r="F9" s="174"/>
+      <c r="G9" s="174"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="174"/>
+      <c r="J9" s="174"/>
+      <c r="K9" s="174"/>
+      <c r="L9" s="175"/>
       <c r="M9" s="107"/>
-      <c r="N9" s="169" t="s">
+      <c r="N9" s="173" t="s">
         <v>89</v>
       </c>
-      <c r="O9" s="171"/>
+      <c r="O9" s="175"/>
       <c r="P9" s="107"/>
       <c r="Q9" s="23" t="s">
         <v>1077</v>
       </c>
       <c r="R9" s="117"/>
-      <c r="S9" s="169" t="s">
+      <c r="S9" s="173" t="s">
         <v>316</v>
       </c>
-      <c r="T9" s="171"/>
+      <c r="T9" s="175"/>
       <c r="U9" s="115"/>
       <c r="V9" s="103"/>
       <c r="W9" s="130"/>
@@ -7779,7 +7779,7 @@
       <c r="Y9" s="130"/>
       <c r="Z9" s="130"/>
     </row>
-    <row r="10" spans="1:26" s="131" customFormat="1" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" s="131" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="74" t="s">
         <v>0</v>
       </c>
@@ -7809,7 +7809,7 @@
       <c r="Y10" s="130"/>
       <c r="Z10" s="130"/>
     </row>
-    <row r="11" spans="1:26" s="133" customFormat="1" ht="41" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" s="133" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="75" t="s">
         <v>85</v>
       </c>
@@ -7870,7 +7870,7 @@
       <c r="Y11" s="136"/>
       <c r="Z11" s="137"/>
     </row>
-    <row r="12" spans="1:26" s="141" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" s="141" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="76" t="s">
         <v>1</v>
       </c>
@@ -7961,7 +7961,7 @@
       <c r="Y13" s="144"/>
       <c r="Z13" s="145"/>
     </row>
-    <row r="14" spans="1:26" s="141" customFormat="1" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" s="141" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="77" t="s">
         <v>2</v>
       </c>
@@ -7997,10 +7997,10 @@
       <c r="B15" s="78" t="s">
         <v>1583</v>
       </c>
-      <c r="C15" s="172" t="s">
+      <c r="C15" s="169" t="s">
         <v>420</v>
       </c>
-      <c r="D15" s="174" t="s">
+      <c r="D15" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E15" s="56" t="s">
@@ -8021,7 +8021,7 @@
       <c r="J15" s="58">
         <v>2</v>
       </c>
-      <c r="K15" s="175" t="s">
+      <c r="K15" s="172" t="s">
         <v>870</v>
       </c>
       <c r="L15" s="58">
@@ -8059,10 +8059,10 @@
       <c r="B16" s="78" t="s">
         <v>1585</v>
       </c>
-      <c r="C16" s="172" t="s">
+      <c r="C16" s="169" t="s">
         <v>421</v>
       </c>
-      <c r="D16" s="174" t="s">
+      <c r="D16" s="171" t="s">
         <v>419</v>
       </c>
       <c r="E16" s="56" t="s">
@@ -8083,7 +8083,7 @@
       <c r="J16" s="58">
         <v>2</v>
       </c>
-      <c r="K16" s="175" t="s">
+      <c r="K16" s="172" t="s">
         <v>79</v>
       </c>
       <c r="L16" s="58">
@@ -8113,10 +8113,10 @@
       <c r="B17" s="78" t="s">
         <v>1587</v>
       </c>
-      <c r="C17" s="172" t="s">
+      <c r="C17" s="169" t="s">
         <v>422</v>
       </c>
-      <c r="D17" s="174" t="s">
+      <c r="D17" s="171" t="s">
         <v>865</v>
       </c>
       <c r="E17" s="56" t="s">
@@ -8135,7 +8135,7 @@
       <c r="J17" s="58">
         <v>2</v>
       </c>
-      <c r="K17" s="174" t="s">
+      <c r="K17" s="171" t="s">
         <v>767</v>
       </c>
       <c r="L17" s="58">
@@ -8165,10 +8165,10 @@
       <c r="B18" s="78" t="s">
         <v>1589</v>
       </c>
-      <c r="C18" s="172" t="s">
+      <c r="C18" s="169" t="s">
         <v>423</v>
       </c>
-      <c r="D18" s="174" t="s">
+      <c r="D18" s="171" t="s">
         <v>871</v>
       </c>
       <c r="E18" s="56" t="s">
@@ -8187,7 +8187,7 @@
       <c r="J18" s="58">
         <v>2</v>
       </c>
-      <c r="K18" s="174" t="s">
+      <c r="K18" s="171" t="s">
         <v>1176</v>
       </c>
       <c r="L18" s="58">
@@ -8217,10 +8217,10 @@
       <c r="B19" s="78" t="s">
         <v>1591</v>
       </c>
-      <c r="C19" s="172" t="s">
+      <c r="C19" s="169" t="s">
         <v>424</v>
       </c>
-      <c r="D19" s="174" t="s">
+      <c r="D19" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E19" s="56" t="s">
@@ -8239,7 +8239,7 @@
       <c r="J19" s="58">
         <v>2</v>
       </c>
-      <c r="K19" s="174" t="s">
+      <c r="K19" s="171" t="s">
         <v>876</v>
       </c>
       <c r="L19" s="58">
@@ -8269,10 +8269,10 @@
       <c r="B20" s="78" t="s">
         <v>1593</v>
       </c>
-      <c r="C20" s="172" t="s">
+      <c r="C20" s="169" t="s">
         <v>425</v>
       </c>
-      <c r="D20" s="174" t="s">
+      <c r="D20" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E20" s="56" t="s">
@@ -8291,7 +8291,7 @@
       <c r="J20" s="58">
         <v>2</v>
       </c>
-      <c r="K20" s="174" t="s">
+      <c r="K20" s="171" t="s">
         <v>1177</v>
       </c>
       <c r="L20" s="58">
@@ -8321,10 +8321,10 @@
       <c r="B21" s="78" t="s">
         <v>1595</v>
       </c>
-      <c r="C21" s="172" t="s">
+      <c r="C21" s="169" t="s">
         <v>426</v>
       </c>
-      <c r="D21" s="174" t="s">
+      <c r="D21" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E21" s="56" t="s">
@@ -8343,7 +8343,7 @@
       <c r="J21" s="58">
         <v>2</v>
       </c>
-      <c r="K21" s="174" t="s">
+      <c r="K21" s="171" t="s">
         <v>1183</v>
       </c>
       <c r="L21" s="58">
@@ -8373,10 +8373,10 @@
       <c r="B22" s="78" t="s">
         <v>1597</v>
       </c>
-      <c r="C22" s="172" t="s">
+      <c r="C22" s="169" t="s">
         <v>427</v>
       </c>
-      <c r="D22" s="174" t="s">
+      <c r="D22" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E22" s="56" t="s">
@@ -8395,7 +8395,7 @@
       <c r="J22" s="58">
         <v>2</v>
       </c>
-      <c r="K22" s="174" t="s">
+      <c r="K22" s="171" t="s">
         <v>1384</v>
       </c>
       <c r="L22" s="58">
@@ -8425,10 +8425,10 @@
       <c r="B23" s="78" t="s">
         <v>1599</v>
       </c>
-      <c r="C23" s="172" t="s">
+      <c r="C23" s="169" t="s">
         <v>428</v>
       </c>
-      <c r="D23" s="174" t="s">
+      <c r="D23" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E23" s="56" t="s">
@@ -8447,7 +8447,7 @@
       <c r="J23" s="58">
         <v>2</v>
       </c>
-      <c r="K23" s="174" t="s">
+      <c r="K23" s="171" t="s">
         <v>1385</v>
       </c>
       <c r="L23" s="58">
@@ -8477,10 +8477,10 @@
       <c r="B24" s="78" t="s">
         <v>1601</v>
       </c>
-      <c r="C24" s="172" t="s">
+      <c r="C24" s="169" t="s">
         <v>429</v>
       </c>
-      <c r="D24" s="174" t="s">
+      <c r="D24" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E24" s="56" t="s">
@@ -8499,7 +8499,7 @@
       <c r="J24" s="58">
         <v>2</v>
       </c>
-      <c r="K24" s="174" t="s">
+      <c r="K24" s="171" t="s">
         <v>974</v>
       </c>
       <c r="L24" s="58">
@@ -8529,10 +8529,10 @@
       <c r="B25" s="78" t="s">
         <v>1603</v>
       </c>
-      <c r="C25" s="173" t="s">
+      <c r="C25" s="170" t="s">
         <v>430</v>
       </c>
-      <c r="D25" s="174" t="s">
+      <c r="D25" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E25" s="56" t="s">
@@ -8551,7 +8551,7 @@
       <c r="J25" s="58">
         <v>2</v>
       </c>
-      <c r="K25" s="175" t="s">
+      <c r="K25" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L25" s="58"/>
@@ -8579,10 +8579,10 @@
       <c r="B26" s="78" t="s">
         <v>1605</v>
       </c>
-      <c r="C26" s="173" t="s">
+      <c r="C26" s="170" t="s">
         <v>431</v>
       </c>
-      <c r="D26" s="174" t="s">
+      <c r="D26" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E26" s="56" t="s">
@@ -8601,7 +8601,7 @@
       <c r="J26" s="58">
         <v>2</v>
       </c>
-      <c r="K26" s="175" t="s">
+      <c r="K26" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L26" s="58"/>
@@ -8629,10 +8629,10 @@
       <c r="B27" s="78" t="s">
         <v>1607</v>
       </c>
-      <c r="C27" s="173" t="s">
+      <c r="C27" s="170" t="s">
         <v>432</v>
       </c>
-      <c r="D27" s="174" t="s">
+      <c r="D27" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E27" s="56" t="s">
@@ -8651,7 +8651,7 @@
       <c r="J27" s="58">
         <v>2</v>
       </c>
-      <c r="K27" s="175" t="s">
+      <c r="K27" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L27" s="58"/>
@@ -8679,10 +8679,10 @@
       <c r="B28" s="78" t="s">
         <v>1609</v>
       </c>
-      <c r="C28" s="173" t="s">
+      <c r="C28" s="170" t="s">
         <v>433</v>
       </c>
-      <c r="D28" s="174" t="s">
+      <c r="D28" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E28" s="56" t="s">
@@ -8701,7 +8701,7 @@
       <c r="J28" s="58">
         <v>2</v>
       </c>
-      <c r="K28" s="175" t="s">
+      <c r="K28" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L28" s="58"/>
@@ -8729,10 +8729,10 @@
       <c r="B29" s="78" t="s">
         <v>1611</v>
       </c>
-      <c r="C29" s="173" t="s">
+      <c r="C29" s="170" t="s">
         <v>434</v>
       </c>
-      <c r="D29" s="174" t="s">
+      <c r="D29" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E29" s="56" t="s">
@@ -8751,7 +8751,7 @@
       <c r="J29" s="58">
         <v>2</v>
       </c>
-      <c r="K29" s="175" t="s">
+      <c r="K29" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L29" s="58"/>
@@ -8779,10 +8779,10 @@
       <c r="B30" s="78" t="s">
         <v>1613</v>
       </c>
-      <c r="C30" s="173" t="s">
+      <c r="C30" s="170" t="s">
         <v>435</v>
       </c>
-      <c r="D30" s="174" t="s">
+      <c r="D30" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E30" s="56" t="s">
@@ -8801,7 +8801,7 @@
       <c r="J30" s="58">
         <v>2</v>
       </c>
-      <c r="K30" s="175" t="s">
+      <c r="K30" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L30" s="58"/>
@@ -8829,10 +8829,10 @@
       <c r="B31" s="78" t="s">
         <v>1615</v>
       </c>
-      <c r="C31" s="173" t="s">
+      <c r="C31" s="170" t="s">
         <v>436</v>
       </c>
-      <c r="D31" s="174" t="s">
+      <c r="D31" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E31" s="56" t="s">
@@ -8851,7 +8851,7 @@
       <c r="J31" s="58">
         <v>2</v>
       </c>
-      <c r="K31" s="175" t="s">
+      <c r="K31" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L31" s="58"/>
@@ -8879,10 +8879,10 @@
       <c r="B32" s="78" t="s">
         <v>1617</v>
       </c>
-      <c r="C32" s="173" t="s">
+      <c r="C32" s="170" t="s">
         <v>437</v>
       </c>
-      <c r="D32" s="174" t="s">
+      <c r="D32" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E32" s="56" t="s">
@@ -8901,7 +8901,7 @@
       <c r="J32" s="58">
         <v>2</v>
       </c>
-      <c r="K32" s="175" t="s">
+      <c r="K32" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L32" s="58"/>
@@ -8929,10 +8929,10 @@
       <c r="B33" s="78" t="s">
         <v>1619</v>
       </c>
-      <c r="C33" s="173" t="s">
+      <c r="C33" s="170" t="s">
         <v>438</v>
       </c>
-      <c r="D33" s="174" t="s">
+      <c r="D33" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E33" s="56" t="s">
@@ -8951,7 +8951,7 @@
       <c r="J33" s="58">
         <v>2</v>
       </c>
-      <c r="K33" s="175" t="s">
+      <c r="K33" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L33" s="58"/>
@@ -8979,10 +8979,10 @@
       <c r="B34" s="78" t="s">
         <v>1621</v>
       </c>
-      <c r="C34" s="173" t="s">
+      <c r="C34" s="170" t="s">
         <v>872</v>
       </c>
-      <c r="D34" s="174" t="s">
+      <c r="D34" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E34" s="56" t="s">
@@ -9001,7 +9001,7 @@
       <c r="J34" s="58">
         <v>2</v>
       </c>
-      <c r="K34" s="175" t="s">
+      <c r="K34" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L34" s="58"/>
@@ -9029,10 +9029,10 @@
       <c r="B35" s="78" t="s">
         <v>1623</v>
       </c>
-      <c r="C35" s="173" t="s">
+      <c r="C35" s="170" t="s">
         <v>873</v>
       </c>
-      <c r="D35" s="174" t="s">
+      <c r="D35" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E35" s="56" t="s">
@@ -9051,7 +9051,7 @@
       <c r="J35" s="58">
         <v>2</v>
       </c>
-      <c r="K35" s="175" t="s">
+      <c r="K35" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L35" s="58"/>
@@ -9079,10 +9079,10 @@
       <c r="B36" s="78" t="s">
         <v>1625</v>
       </c>
-      <c r="C36" s="173" t="s">
+      <c r="C36" s="170" t="s">
         <v>874</v>
       </c>
-      <c r="D36" s="174" t="s">
+      <c r="D36" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E36" s="56" t="s">
@@ -9101,7 +9101,7 @@
       <c r="J36" s="58">
         <v>2</v>
       </c>
-      <c r="K36" s="175" t="s">
+      <c r="K36" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L36" s="58"/>
@@ -9129,10 +9129,10 @@
       <c r="B37" s="78" t="s">
         <v>1627</v>
       </c>
-      <c r="C37" s="173" t="s">
+      <c r="C37" s="170" t="s">
         <v>875</v>
       </c>
-      <c r="D37" s="174" t="s">
+      <c r="D37" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E37" s="56" t="s">
@@ -9151,7 +9151,7 @@
       <c r="J37" s="58">
         <v>2</v>
       </c>
-      <c r="K37" s="175" t="s">
+      <c r="K37" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L37" s="58"/>
@@ -9179,10 +9179,10 @@
       <c r="B38" s="78" t="s">
         <v>1629</v>
       </c>
-      <c r="C38" s="173" t="s">
+      <c r="C38" s="170" t="s">
         <v>864</v>
       </c>
-      <c r="D38" s="174" t="s">
+      <c r="D38" s="171" t="s">
         <v>278</v>
       </c>
       <c r="E38" s="56" t="s">
@@ -9201,7 +9201,7 @@
       <c r="J38" s="58">
         <v>2</v>
       </c>
-      <c r="K38" s="175" t="s">
+      <c r="K38" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L38" s="58"/>
@@ -9225,7 +9225,7 @@
     <row r="39" spans="1:26" s="151" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="100"/>
       <c r="B39" s="78"/>
-      <c r="C39" s="173" t="s">
+      <c r="C39" s="170" t="s">
         <v>1579</v>
       </c>
       <c r="D39" s="60"/>
@@ -9245,7 +9245,7 @@
       <c r="J39" s="58">
         <v>2</v>
       </c>
-      <c r="K39" s="175" t="s">
+      <c r="K39" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L39" s="58"/>
@@ -9269,7 +9269,7 @@
     <row r="40" spans="1:26" s="151" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="100"/>
       <c r="B40" s="78"/>
-      <c r="C40" s="173" t="s">
+      <c r="C40" s="170" t="s">
         <v>1580</v>
       </c>
       <c r="D40" s="60"/>
@@ -9289,7 +9289,7 @@
       <c r="J40" s="58">
         <v>2</v>
       </c>
-      <c r="K40" s="175" t="s">
+      <c r="K40" s="172" t="s">
         <v>80</v>
       </c>
       <c r="L40" s="58"/>
@@ -20059,7 +20059,7 @@
       <c r="T399" s="163"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LcEW3xxqy8+uxIfecIYabamdN8eTKoPpDyQutSviBMF83dE15eAIw/7xf88mxehDeKVO0pK6Sirr6CzoHnWduw==" saltValue="phe6gu6JQS2q2aNlfVxepQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="N9:O9"/>

</xml_diff>